<commit_message>
added new images and code
</commit_message>
<xml_diff>
--- a/app/training_data.xlsx
+++ b/app/training_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagar.patel\OneDrive - Centric Consulting\Documents\GitHub\ChatBot\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E982E9-33AC-449A-8CB6-AC35ACC05515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A529E3CC-B200-4796-96FB-5FE1426FA7BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6D91F609-99E5-D24F-92A5-78FDD7B3F1B9}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>input</t>
   </si>
@@ -79,9 +79,6 @@
     <t>Goodevening, I am your centric Buddy how can I help you today ?</t>
   </si>
   <si>
-    <t xml:space="preserve">Welcome to Centric consulting </t>
-  </si>
-  <si>
     <t xml:space="preserve">about centric </t>
   </si>
   <si>
@@ -98,6 +95,9 @@
   </si>
   <si>
     <t>calculate A+B or A*b or A/B</t>
+  </si>
+  <si>
+    <t>Welcome to Centric consulting, I am your centric Buddy how can I help you today ?</t>
   </si>
 </sst>
 </file>
@@ -139,7 +139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -151,13 +151,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,19 +471,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EA67215-5E8D-4750-B3F5-22A69B5AA4C1}">
-  <dimension ref="A1:B91"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="G11" sqref="G11:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.08203125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="74.08203125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="36.08203125" customWidth="1"/>
+    <col min="2" max="2" width="74.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -492,7 +491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -500,7 +499,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -508,7 +507,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -516,7 +515,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
@@ -524,7 +523,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
@@ -532,127 +531,129 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="5"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+      <c r="B8" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+      <c r="B11" s="5"/>
+      <c r="G11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="5"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
+    </row>
+    <row r="12" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+      <c r="B12" s="5"/>
+      <c r="G12" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+      <c r="B13" s="5"/>
+      <c r="G13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="5"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
+    </row>
+    <row r="14" spans="1:7" ht="93" x14ac:dyDescent="0.35">
+      <c r="B14" s="5"/>
+      <c r="G14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="5"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
+    </row>
+    <row r="15" spans="1:7" ht="108.5" x14ac:dyDescent="0.35">
+      <c r="B15" s="5"/>
+      <c r="G15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="5"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="5"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="5"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="5"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G16" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="62" x14ac:dyDescent="0.35">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G17" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="2"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
       <c r="B32" s="2"/>
     </row>

</xml_diff>